<commit_message>
Adding README.md and LICENSE.md before publishing to GitHub
</commit_message>
<xml_diff>
--- a/docs/data_generator_template.xlsx
+++ b/docs/data_generator_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Custom project information" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="288">
   <si>
     <t>Tag Naming Convention</t>
   </si>
@@ -367,9 +367,6 @@
     <t>PHP Shared Library</t>
   </si>
   <si>
-    <t>php_shared_libary_v</t>
-  </si>
-  <si>
     <t>DB DDL Helper</t>
   </si>
   <si>
@@ -847,9 +844,6 @@
     <t>https://picgitlab.nmfs.local/centralized-data-tools/centralized-ctd/-/blob/master/CDIM/docs/CTD%20Data%20Import%20Module%20-%20Technical%20Documentation.md</t>
   </si>
   <si>
-    <t>https://picgitlab.nmfs.local/centralized-data-tools/parr-tools/-/blob/master/docs/PIFSC%20Data%20Set%20Database%20Documentation.docx</t>
-  </si>
-  <si>
     <t>https://picgitlab.nmfs.local/centralized-data-tools/parr-tools/-/blob/master/bulk_download/docs/Bulk%20Download%20Module%20Documentation.docx</t>
   </si>
   <si>
@@ -929,6 +923,27 @@
   </si>
   <si>
     <t>PGL</t>
+  </si>
+  <si>
+    <t>Metadata Tool</t>
+  </si>
+  <si>
+    <t>data_mgmt_plan_app_v</t>
+  </si>
+  <si>
+    <t>Data Management Plan (DMP) App</t>
+  </si>
+  <si>
+    <t>https://picgitlab.nmfs.local/data-enterprise/data-management-plan-app/-/blob/main/docs/Data%20Management%20Plan%20App%20Technical%20Documentation.md</t>
+  </si>
+  <si>
+    <t>This Data Management Plan (DMP) App (DMPA) project was developed to generate a formatted DMP in Google Doc and PDF formats when the corresponding DMP Form is submitted. There are three different versions of the DMPA that were developed to demonstrate the potential functionality based on the project sponsor's guidance.</t>
+  </si>
+  <si>
+    <t>php_shared_library_v</t>
+  </si>
+  <si>
+    <t>https://picgitlab.nmfs.local/centralized-data-tools/parr-tools/-/blob/master/docs/PIR%20Data%20Set%20Database%20Documentation.md</t>
   </si>
 </sst>
 </file>
@@ -1303,9 +1318,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1323,13 +1340,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -1338,19 +1355,19 @@
         <v>6</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1358,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1373,10 +1390,10 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J2" s="1" t="str">
         <f t="shared" ref="J2:J16" si="0">"{""tag_naming_convention"": """&amp;D2&amp;""", ""resource_scope"":"""&amp;B2&amp;""", ""resource_name"": """&amp;E2&amp;""", ""resource_description"": """&amp;SUBSTITUTE(H2, """", """""")&amp;""", ""resource_type"": """&amp;C2&amp;""", ""resource_category"": """&amp;A2&amp;""", ""project_color"": """&amp;F2&amp;""", ""resource_url"":"""&amp;G2&amp;""", ""demo_url"":"""&amp;I2&amp;"""}"</f>
@@ -1388,7 +1405,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1403,10 +1420,10 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1418,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1433,10 +1450,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1448,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
@@ -1466,7 +1483,7 @@
         <v>37</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1478,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -1496,7 +1513,7 @@
         <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1508,7 +1525,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
@@ -1526,7 +1543,7 @@
         <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1538,25 +1555,25 @@
         <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1568,7 +1585,7 @@
         <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -1583,10 +1600,10 @@
         <v>36</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1598,28 +1615,28 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1631,7 +1648,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>3</v>
@@ -1649,7 +1666,7 @@
         <v>40</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1661,7 +1678,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
@@ -1679,7 +1696,7 @@
         <v>43</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1691,7 +1708,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>3</v>
@@ -1706,10 +1723,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1721,28 +1738,28 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="I14" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1754,7 +1771,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -1769,10 +1786,10 @@
         <v>18</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1784,7 +1801,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
@@ -1799,13 +1816,13 @@
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1817,7 +1834,7 @@
         <v>55</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
@@ -1832,10 +1849,10 @@
         <v>20</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" ref="J17:J49" si="1">"{""tag_naming_convention"": """&amp;D17&amp;""", ""resource_scope"":"""&amp;B17&amp;""", ""resource_name"": """&amp;E17&amp;""", ""resource_description"": """&amp;SUBSTITUTE(H17, """", """""")&amp;""", ""resource_type"": """&amp;C17&amp;""", ""resource_category"": """&amp;A17&amp;""", ""project_color"": """&amp;F17&amp;""", ""resource_url"":"""&amp;G17&amp;""", ""demo_url"":"""&amp;I17&amp;"""}"</f>
@@ -1847,7 +1864,7 @@
         <v>62</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
@@ -1862,10 +1879,10 @@
         <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1877,7 +1894,7 @@
         <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1892,13 +1909,13 @@
         <v>35</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1910,7 +1927,7 @@
         <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -1925,10 +1942,10 @@
         <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1940,7 +1957,7 @@
         <v>71</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
@@ -1955,10 +1972,10 @@
         <v>15</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1970,7 +1987,7 @@
         <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>1</v>
@@ -1985,10 +2002,10 @@
         <v>16</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2000,7 +2017,7 @@
         <v>81</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>1</v>
@@ -2015,10 +2032,10 @@
         <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2030,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
@@ -2045,10 +2062,10 @@
         <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2060,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>3</v>
@@ -2069,16 +2086,16 @@
         <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2090,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>1</v>
@@ -2105,10 +2122,10 @@
         <v>36</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2120,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
@@ -2135,10 +2152,10 @@
         <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2150,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
@@ -2165,13 +2182,13 @@
         <v>46</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2183,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
@@ -2198,10 +2215,10 @@
         <v>17</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2213,7 +2230,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
@@ -2228,10 +2245,10 @@
         <v>18</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J30" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2243,7 +2260,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>3</v>
@@ -2258,10 +2275,10 @@
         <v>19</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J31" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2273,13 +2290,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
+        <v>286</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>94</v>
@@ -2288,14 +2305,14 @@
         <v>20</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>{"tag_naming_convention": "php_shared_libary_v", "resource_scope":"SW", "resource_name": "PHP Shared Library", "resource_description": "The PHP Shared Library was developed to provide reusable classes/functions that provide functionality that is used in multiple modules/applications. Each file contains one or more functions or a single PHP class that can be included in any new or existing PHP project. These files are available to help developers spend time focusing on the development of specific features particular to their specific applications instead of common functionality that is used in multiple applications. The intent was to continue to develop these shared code files as more functionality was required for PHP projects. Some of these files contain simple wrappers for existing functions (e.g. mssql_connect) or more complex classes (e.g. output_message) or functions (find_array_pos).", "resource_type": "Tool", "resource_category": "Development Tool", "project_color": "#CCCCFF", "resource_url":"https://picgitlab.nmfs.local/centralized-data-tools/php-shared-library/-/blob/master/docs/PHP%20Shared%20Library%20Technical%20Documentation.md", "demo_url":""}</v>
+        <v>{"tag_naming_convention": "php_shared_library_v", "resource_scope":"SW", "resource_name": "PHP Shared Library", "resource_description": "The PHP Shared Library was developed to provide reusable classes/functions that provide functionality that is used in multiple modules/applications. Each file contains one or more functions or a single PHP class that can be included in any new or existing PHP project. These files are available to help developers spend time focusing on the development of specific features particular to their specific applications instead of common functionality that is used in multiple applications. The intent was to continue to develop these shared code files as more functionality was required for PHP projects. Some of these files contain simple wrappers for existing functions (e.g. mssql_connect) or more complex classes (e.g. output_message) or functions (find_array_pos).", "resource_type": "Tool", "resource_category": "Development Tool", "project_color": "#CCCCFF", "resource_url":"https://picgitlab.nmfs.local/centralized-data-tools/php-shared-library/-/blob/master/docs/PHP%20Shared%20Library%20Technical%20Documentation.md", "demo_url":""}</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2303,28 +2320,28 @@
         <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2336,25 +2353,25 @@
         <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2366,25 +2383,25 @@
         <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2396,25 +2413,25 @@
         <v>81</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2426,28 +2443,28 @@
         <v>81</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2459,25 +2476,25 @@
         <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2486,58 +2503,58 @@
     </row>
     <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>{"tag_naming_convention": "PIFSC_Data_Set_db_v", "resource_scope":"DS", "resource_name": "PIFSC Data Set Database (DSD)", "resource_description": "The PIFSC Data Set Database (DSD) was developed to facilitate the dissemination and archival of scientific data sets to satisfy PARR requirements.  There were multiple PARR software modules developed by PIFSC to facilitate PARR compliance for the Science Center.  The PIFSC PARR modules are the Bulk Download Module (BDM), the APEX Data Set Information Application (DSIA), and the Data Set URL Verification Module (UVM)", "resource_type": "Tool", "resource_category": "PARR Compliance Tools", "project_color": "#00FFDD", "resource_url":"https://picgitlab.nmfs.local/centralized-data-tools/parr-tools/-/blob/master/docs/PIFSC%20Data%20Set%20Database%20Documentation.docx", "demo_url":""}</v>
+        <v>{"tag_naming_convention": "PIFSC_Data_Set_db_v", "resource_scope":"DS", "resource_name": "PIFSC Data Set Database (DSD)", "resource_description": "The PIFSC Data Set Database (DSD) was developed to facilitate the dissemination and archival of scientific data sets to satisfy PARR requirements.  There were multiple PARR software modules developed by PIFSC to facilitate PARR compliance for the Science Center.  The PIFSC PARR modules are the Bulk Download Module (BDM), the APEX Data Set Information Application (DSIA), and the Data Set URL Verification Module (UVM)", "resource_type": "Tool", "resource_category": "PARR Compliance Tools", "project_color": "#00FFDD", "resource_url":"https://picgitlab.nmfs.local/centralized-data-tools/parr-tools/-/blob/master/docs/PIR%20Data%20Set%20Database%20Documentation.md", "demo_url":""}</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J40" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2546,31 +2563,31 @@
     </row>
     <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I41" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="J41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2579,28 +2596,28 @@
     </row>
     <row r="42" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J42" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2609,25 +2626,25 @@
     </row>
     <row r="43" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2636,25 +2653,25 @@
     </row>
     <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="J44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2663,22 +2680,22 @@
     </row>
     <row r="45" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2687,22 +2704,22 @@
     </row>
     <row r="46" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J46" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2711,22 +2728,22 @@
     </row>
     <row r="47" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2735,25 +2752,25 @@
     </row>
     <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="J48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2762,25 +2779,25 @@
     </row>
     <row r="49" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="J49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2789,43 +2806,43 @@
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J51" s="1"/>
     </row>
@@ -2834,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>3</v>
@@ -2848,6 +2865,33 @@
       <c r="J52" s="1" t="str">
         <f>"{""tag_naming_convention"": """&amp;D52&amp;""", ""resource_scope"":"""&amp;B52&amp;""", ""resource_name"": """&amp;E52&amp;""", ""resource_description"": """&amp;SUBSTITUTE(H52, """", """""")&amp;""", ""resource_type"": """&amp;C52&amp;""", ""resource_category"": """&amp;A52&amp;""", ""project_color"": """&amp;F52&amp;""", ""resource_url"":"""&amp;G52&amp;""", ""demo_url"":"""&amp;I52&amp;"""}"</f>
         <v>{"tag_naming_convention": "", "resource_scope":"SW", "resource_name": "Data History Tracking Package", "resource_description": "", "resource_type": "Tool", "resource_category": "Development Tool", "project_color": "#00FFDD", "resource_url":"", "demo_url":""}</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>282</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G53" t="s">
+        <v>284</v>
+      </c>
+      <c r="H53" t="s">
+        <v>285</v>
+      </c>
+      <c r="J53" s="1" t="str">
+        <f>"{""tag_naming_convention"": """&amp;D53&amp;""", ""resource_scope"":"""&amp;B53&amp;""", ""resource_name"": """&amp;E53&amp;""", ""resource_description"": """&amp;SUBSTITUTE(H53, """", """""")&amp;""", ""resource_type"": """&amp;C53&amp;""", ""resource_category"": """&amp;A53&amp;""", ""project_color"": """&amp;F53&amp;""", ""resource_url"":"""&amp;G53&amp;""", ""demo_url"":"""&amp;I53&amp;"""}"</f>
+        <v>{"tag_naming_convention": "data_mgmt_plan_app_v", "resource_scope":"DS", "resource_name": "Data Management Plan (DMP) App", "resource_description": "This Data Management Plan (DMP) App (DMPA) project was developed to generate a formatted DMP in Google Doc and PDF formats when the corresponding DMP Form is submitted. There are three different versions of the DMPA that were developed to demonstrate the potential functionality based on the project sponsor's guidance.", "resource_type": "Tool", "resource_category": "Metadata Tool", "project_color": "", "resource_url":"https://picgitlab.nmfs.local/data-enterprise/data-management-plan-app/-/blob/main/docs/Data%20Management%20Plan%20App%20Technical%20Documentation.md", "demo_url":""}</v>
       </c>
     </row>
   </sheetData>
@@ -2924,13 +2968,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D7" si="0">"INSERT INTO PRI_RES_TYPES ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A4, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B4, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C4, "'", "''")&amp;"');"</f>
@@ -2939,13 +2983,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" t="s">
         <v>189</v>
-      </c>
-      <c r="C5" t="s">
-        <v>190</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -2954,13 +2998,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -2969,13 +3013,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -3018,7 +3062,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3033,13 +3077,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
         <v>213</v>
-      </c>
-      <c r="C3" t="s">
-        <v>214</v>
       </c>
       <c r="D3" t="str">
         <f>"INSERT INTO PRI_RES_SCOPES ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C3, "'", "''")&amp;"');"</f>
@@ -3048,13 +3092,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="s">
         <v>191</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>193</v>
       </c>
       <c r="D4" t="str">
         <f>"INSERT INTO PRI_RES_SCOPES ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A4, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B4, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C4, "'", "''")&amp;"');"</f>
@@ -3071,7 +3115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3084,13 +3128,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
         <v>272</v>
-      </c>
-      <c r="B1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" t="s">
-        <v>274</v>
       </c>
       <c r="D1" t="s">
         <v>32</v>
@@ -3098,10 +3142,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -3113,28 +3157,28 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D7" si="0">"INSERT INTO PRI_DATA_SOURCES ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C3, "'", "''")&amp;"');"</f>
+        <f t="shared" ref="D3:D4" si="0">"INSERT INTO PRI_DATA_SOURCES ("&amp;$A$1&amp;", "&amp;$B$1&amp;", "&amp;$C$1&amp;") VALUES ('"&amp;SUBSTITUTE(A3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(B3, "'", "''")&amp;"', '"&amp;SUBSTITUTE(C3, "'", "''")&amp;"');"</f>
         <v>INSERT INTO PRI_DATA_SOURCES (DATA_SOURCE_CODE, DATA_SOURCE_NAME, DATA_SOURCE_DESC) VALUES ('PGL', 'PIFSC GitLab', 'On-prem GitLab instance hosted by PIFSC');</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>

</xml_diff>